<commit_message>
Correct issue with loading empty packages after splitting the list of packages.
</commit_message>
<xml_diff>
--- a/ExcelRAddIn/Tests/Forecast.xlsx
+++ b/ExcelRAddIn/Tests/Forecast.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\C#\Office\Office365 AddIns\ExcelRAddIn\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A98C7CC-69BB-41B5-A6C7-6C031F2A82C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7232AD9F-730C-4A92-B5F2-BBA7BD9C3596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="899" firstSheet="9" activeTab="18" xr2:uid="{237949DD-86ED-4837-BFB0-873A1F9330BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="899" activeTab="9" xr2:uid="{237949DD-86ED-4837-BFB0-873A1F9330BE}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="2" r:id="rId1"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -966,9 +966,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -985,6 +982,9 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4424,7 +4424,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D562DCAA-9A4E-4A3E-8308-7D30612CCEAE}">
   <dimension ref="B2:EX32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4434,10 +4436,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="J2" s="10" t="s">
         <v>28</v>
       </c>
@@ -4702,13 +4704,13 @@
       </c>
     </row>
     <row r="19" spans="2:154" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>191</v>
       </c>
       <c r="J19" t="str">
@@ -5348,10 +5350,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="J2" s="10" t="s">
         <v>28</v>
       </c>
@@ -6002,10 +6004,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="H2" s="7" t="s">
         <v>28</v>
       </c>
@@ -7682,10 +7684,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:O2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -8935,10 +8937,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:84" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:O2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -10726,10 +10728,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:P2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -11062,10 +11064,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:N2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>model</v>
@@ -11948,10 +11950,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="37"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
@@ -11993,15 +11995,15 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="J6" s="16"/>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
@@ -12011,26 +12013,26 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="J7" s="16"/>
-      <c r="K7" s="32" t="str" cm="1">
+      <c r="K7" s="31" t="str" cm="1">
         <f t="array" ref="K7:Q8">_xll.Model.Accuracy(C8)</f>
         <v>Index</v>
       </c>
-      <c r="L7" s="33" t="str">
+      <c r="L7" s="32" t="str">
         <v>ME</v>
       </c>
-      <c r="M7" s="33" t="str">
+      <c r="M7" s="32" t="str">
         <v>RMSE</v>
       </c>
-      <c r="N7" s="33" t="str">
+      <c r="N7" s="32" t="str">
         <v>MAE</v>
       </c>
-      <c r="O7" s="33" t="str">
+      <c r="O7" s="32" t="str">
         <v>MPE</v>
       </c>
-      <c r="P7" s="33" t="str">
+      <c r="P7" s="32" t="str">
         <v>MAPE</v>
       </c>
-      <c r="Q7" s="33" t="str">
+      <c r="Q7" s="32" t="str">
         <v>MASE</v>
       </c>
     </row>
@@ -12048,25 +12050,25 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="J8" s="16"/>
-      <c r="K8" s="34" t="str">
+      <c r="K8" s="33" t="str">
         <v>Training set</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="34">
         <v>-2.3728125945569426E-16</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="34">
         <v>54.534506468374872</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="34">
         <v>40.47955300968804</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="34">
         <v>-75.33900029820343</v>
       </c>
-      <c r="P8" s="35">
+      <c r="P8" s="34">
         <v>251.9938767537096</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="34">
         <v>0.49449734925101435</v>
       </c>
     </row>
@@ -12118,22 +12120,22 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="K11" s="30" t="str">
+      <c r="K11" s="29" t="str">
         <v>Area</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="30">
         <v>1</v>
       </c>
-      <c r="M11" s="31">
+      <c r="M11" s="30">
         <v>145465.08832562366</v>
       </c>
-      <c r="N11" s="31">
+      <c r="N11" s="30">
         <v>145465.08832562366</v>
       </c>
-      <c r="O11" s="31">
+      <c r="O11" s="30">
         <v>39.129652192045477</v>
       </c>
-      <c r="P11" s="31">
+      <c r="P11" s="30">
         <v>1.8246037566969249E-6</v>
       </c>
     </row>
@@ -12146,22 +12148,22 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="K12" s="30" t="str">
+      <c r="K12" s="29" t="str">
         <v>Elevation</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="30">
         <v>1</v>
       </c>
-      <c r="M12" s="31">
+      <c r="M12" s="30">
         <v>65666.629692837261</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="30">
         <v>65666.629692837261</v>
       </c>
-      <c r="O12" s="31">
+      <c r="O12" s="30">
         <v>17.664117281204366</v>
       </c>
-      <c r="P12" s="31">
+      <c r="P12" s="30">
         <v>3.1520105175534223E-4</v>
       </c>
     </row>
@@ -12174,22 +12176,22 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="K13" s="30" t="str">
+      <c r="K13" s="29" t="str">
         <v>Nearest</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="30">
         <v>1</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="30">
         <v>29.309994088102041</v>
       </c>
-      <c r="N13" s="31">
+      <c r="N13" s="30">
         <v>29.309994088102041</v>
       </c>
-      <c r="O13" s="31">
+      <c r="O13" s="30">
         <v>7.8842964151716495E-3</v>
       </c>
-      <c r="P13" s="31">
+      <c r="P13" s="30">
         <v>0.92998278059540307</v>
       </c>
     </row>
@@ -12203,22 +12205,22 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="17"/>
-      <c r="K14" s="30" t="str">
+      <c r="K14" s="29" t="str">
         <v>Scruz</v>
       </c>
-      <c r="L14" s="31">
+      <c r="L14" s="30">
         <v>1</v>
       </c>
-      <c r="M14" s="31">
+      <c r="M14" s="30">
         <v>14278.485641368316</v>
       </c>
-      <c r="N14" s="31">
+      <c r="N14" s="30">
         <v>14278.485641368316</v>
       </c>
-      <c r="O14" s="31">
+      <c r="O14" s="30">
         <v>3.8408678220108738</v>
       </c>
-      <c r="P14" s="31">
+      <c r="P14" s="30">
         <v>6.1729080849071229E-2</v>
       </c>
     </row>
@@ -12231,22 +12233,22 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="K15" s="30" t="str">
+      <c r="K15" s="29" t="str">
         <v>Adjacent</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="30">
         <v>1</v>
       </c>
-      <c r="M15" s="31">
+      <c r="M15" s="30">
         <v>66421.481140272663</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="30">
         <v>66421.481140272663</v>
       </c>
-      <c r="O15" s="31">
+      <c r="O15" s="30">
         <v>17.867169951331583</v>
       </c>
-      <c r="P15" s="31">
+      <c r="P15" s="30">
         <v>2.9650744889825993E-4</v>
       </c>
     </row>
@@ -12259,22 +12261,22 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
-      <c r="K16" s="30" t="str">
+      <c r="K16" s="29" t="str">
         <v>Residuals</v>
       </c>
-      <c r="L16" s="31">
+      <c r="L16" s="30">
         <v>24</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M16" s="30">
         <v>89220.371872476637</v>
       </c>
-      <c r="N16" s="31">
+      <c r="N16" s="30">
         <v>3717.5154946865264</v>
       </c>
-      <c r="O16" s="31" t="str">
+      <c r="O16" s="30" t="str">
         <v/>
       </c>
-      <c r="P16" s="31" t="str">
+      <c r="P16" s="30" t="str">
         <v/>
       </c>
     </row>
@@ -12326,10 +12328,10 @@
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="L20" s="37"/>
+      <c r="L20" s="36"/>
       <c r="M20" s="14"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
@@ -12341,7 +12343,7 @@
         <f t="array" ref="K21:M34">_xll.RScript.Params("lm", TRUE, TRUE)</f>
         <v>formula</v>
       </c>
-      <c r="L21" s="30" t="str">
+      <c r="L21" s="29" t="str">
         <v>symbol</v>
       </c>
       <c r="M21" s="14" t="str">
@@ -12990,10 +12992,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="37"/>
       <c r="F3" s="10" t="s">
         <v>28</v>
       </c>
@@ -14458,10 +14460,10 @@
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="25"/>
+      <c r="C46" s="37"/>
       <c r="R46" t="str">
         <v xml:space="preserve">        if (is.factor(y)) {</v>
       </c>
@@ -14701,7 +14703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9135BF-2115-4D96-AD2D-B561EFF71C80}">
   <dimension ref="B2:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25418,7 +25420,7 @@
   <dimension ref="B2:P185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25429,14 +25431,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="O2" s="25" t="s">
+      <c r="E2" s="37"/>
+      <c r="O2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="25"/>
+      <c r="P2" s="37"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D3" s="3" t="s">
@@ -27112,10 +27114,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
@@ -27733,10 +27735,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="E2" s="10" t="s">
         <v>28</v>
       </c>
@@ -28873,15 +28875,15 @@
       <c r="B5" s="10"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
@@ -29574,10 +29576,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="37"/>
       <c r="E2" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added enhanced support for ggplot creation - Phase 1
</commit_message>
<xml_diff>
--- a/ExcelRAddIn/Tests/Forecast.xlsx
+++ b/ExcelRAddIn/Tests/Forecast.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\C#\Office\Office365 AddIns\ExcelRAddIn\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE3E099-08D8-4A3F-9808-C4AF6A4E0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F116623-D71E-40C6-A6D9-47C4385813E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="899" firstSheet="8" activeTab="17" xr2:uid="{237949DD-86ED-4837-BFB0-873A1F9330BE}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="899" activeTab="1" xr2:uid="{237949DD-86ED-4837-BFB0-873A1F9330BE}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="2" r:id="rId1"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="198">
   <si>
     <t>Day</t>
   </si>
@@ -805,6 +805,43 @@
   <si>
     <t>Arima</t>
   </si>
+  <si>
+    <t>library(ggplot2)</t>
+  </si>
+  <si>
+    <t>library(ggthemes)</t>
+  </si>
+  <si>
+    <t># Convert AirPassengers time series to a data frame</t>
+  </si>
+  <si>
+    <t>data &lt;- data.frame(
+  Year = time(AirPassengers),
+  Passengers = as.numeric(AirPassengers)
+)</t>
+  </si>
+  <si>
+    <t>plot(
+	ggplot(data = data, mapping = aes(x = Year, y = Passengers, )) + 
+	geom_line(colour = 'blue') + 
+	theme_minimal() + 
+	labs(title = 'Monthly Airline Passenger Numbers (1949-1960)', x = 'Year', y = 'Number of Passengers', )
+)</t>
+  </si>
+  <si>
+    <t>plot(
+	ggplot(data = mpg, mapping = aes(x = displ, y = hwy)) + 
+geom_point()
+)</t>
+  </si>
+  <si>
+    <t>plot(
+ggplot(data = data, mapping = aes(x = Year, y = Passengers)) + 
+geom_line(colour = 'blue', linetype = 'dotted') + 
+	labs(title = 'Monthly Airline Passenger Numbers (1949-1960)', x = 'Year', y = 'Number of Passengers', caption = 'Dataset') + 
+theme_minimal()
+)</t>
+  </si>
 </sst>
 </file>
 
@@ -920,7 +957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -957,6 +994,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4392,10 +4432,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="J2" s="10" t="s">
         <v>28</v>
       </c>
@@ -5047,10 +5087,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="H2" s="7" t="s">
         <v>28</v>
       </c>
@@ -6777,10 +6817,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:O2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -8030,10 +8070,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:84" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:O2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -9821,10 +9861,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:P2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -10155,10 +10195,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:N2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>model</v>
@@ -11041,10 +11081,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
@@ -12033,7 +12073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F812DA7-7958-4E93-99D4-1625C4C8E1B7}">
   <dimension ref="B3:AP64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -12048,10 +12088,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="27"/>
       <c r="F3" s="10" t="s">
         <v>28</v>
       </c>
@@ -13516,10 +13556,10 @@
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="26"/>
+      <c r="C46" s="27"/>
       <c r="R46" t="str">
         <v xml:space="preserve">        if (is.factor(y)) {</v>
       </c>
@@ -14849,15 +14889,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA1CB6E-EEA6-410B-8C3F-D152623D3978}">
-  <dimension ref="C2:E3"/>
+  <dimension ref="C2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.3">
@@ -14876,6 +14916,64 @@
       <c r="E3" t="str" cm="1">
         <f t="array" ref="E3">_xll.RScript.Evaluate(C3, TRUE)</f>
         <v>OK</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="str" cm="1">
+        <f t="array" ref="E4">_xll.RScript.Evaluate(C4, TRUE)</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" t="str" cm="1">
+        <f t="array" ref="E5">_xll.RScript.Evaluate(C5, TRUE)</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="26"/>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C11" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" t="str" cm="1">
+        <f t="array" ref="E11">_xll.RScript.Evaluate(C11, TRUE)</f>
+        <v>data</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="C13" s="26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C16" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" t="str" cm="1">
+        <f t="array" ref="E16">_xll.RScript.Evaluate(C16, TRUE)</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C19" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" cm="1">
+        <f t="array" aca="1" ref="E19" ca="1">_xll.RScript.Evaluate(C19, TRUE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -14887,7 +14985,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16A5A11-FD74-4F49-8237-7EB8CA3CF65D}">
   <dimension ref="B2:AJ1110"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -24386,14 +24486,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="O2" s="26" t="s">
+      <c r="E2" s="27"/>
+      <c r="O2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="26"/>
+      <c r="P2" s="27"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D3" s="3" t="s">
@@ -26069,10 +26169,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
@@ -26692,10 +26792,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="E2" s="10" t="s">
         <v>28</v>
       </c>
@@ -27833,15 +27933,15 @@
       <c r="B5" s="10"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="26"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
@@ -28534,10 +28634,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="E2" t="s">
         <v>28</v>
       </c>
@@ -29634,10 +29734,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="J2" s="10" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Development to support generating ggplot script.
</commit_message>
<xml_diff>
--- a/ExcelRAddIn/Tests/Forecast.xlsx
+++ b/ExcelRAddIn/Tests/Forecast.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\C#\Office\Office365 AddIns\ExcelRAddIn\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F116623-D71E-40C6-A6D9-47C4385813E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32271BFD-36EA-47F6-A842-EE4AAF22C8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="899" activeTab="1" xr2:uid="{237949DD-86ED-4837-BFB0-873A1F9330BE}"/>
   </bookViews>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="193">
   <si>
     <t>Day</t>
   </si>
@@ -811,37 +811,6 @@
   <si>
     <t>library(ggthemes)</t>
   </si>
-  <si>
-    <t># Convert AirPassengers time series to a data frame</t>
-  </si>
-  <si>
-    <t>data &lt;- data.frame(
-  Year = time(AirPassengers),
-  Passengers = as.numeric(AirPassengers)
-)</t>
-  </si>
-  <si>
-    <t>plot(
-	ggplot(data = data, mapping = aes(x = Year, y = Passengers, )) + 
-	geom_line(colour = 'blue') + 
-	theme_minimal() + 
-	labs(title = 'Monthly Airline Passenger Numbers (1949-1960)', x = 'Year', y = 'Number of Passengers', )
-)</t>
-  </si>
-  <si>
-    <t>plot(
-	ggplot(data = mpg, mapping = aes(x = displ, y = hwy)) + 
-geom_point()
-)</t>
-  </si>
-  <si>
-    <t>plot(
-ggplot(data = data, mapping = aes(x = Year, y = Passengers)) + 
-geom_line(colour = 'blue', linetype = 'dotted') + 
-	labs(title = 'Monthly Airline Passenger Numbers (1949-1960)', x = 'Year', y = 'Number of Passengers', caption = 'Dataset') + 
-theme_minimal()
-)</t>
-  </si>
 </sst>
 </file>
 
@@ -957,7 +926,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -994,9 +963,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4382,7 +4348,7 @@
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4432,10 +4398,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="J2" s="10" t="s">
         <v>28</v>
       </c>
@@ -5087,10 +5053,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="H2" s="7" t="s">
         <v>28</v>
       </c>
@@ -6817,10 +6783,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:O2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -8070,10 +8036,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:84" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:O2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -9861,10 +9827,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:P2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>method</v>
@@ -10195,10 +10161,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:N2">TRANSPOSE(_xll.Model.Results(C9))</f>
         <v>model</v>
@@ -11081,10 +11047,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
@@ -12088,10 +12054,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="26"/>
       <c r="F3" s="10" t="s">
         <v>28</v>
       </c>
@@ -13556,10 +13522,10 @@
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="27"/>
+      <c r="C46" s="26"/>
       <c r="R46" t="str">
         <v xml:space="preserve">        if (is.factor(y)) {</v>
       </c>
@@ -14889,15 +14855,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA1CB6E-EEA6-410B-8C3F-D152623D3978}">
-  <dimension ref="C2:E19"/>
+  <dimension ref="C2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="59.109375" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.3">
@@ -14934,46 +14900,6 @@
       <c r="E5" t="str" cm="1">
         <f t="array" ref="E5">_xll.RScript.Evaluate(C5, TRUE)</f>
         <v>OK</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="26"/>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C11" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="E11" t="str" cm="1">
-        <f t="array" ref="E11">_xll.RScript.Evaluate(C11, TRUE)</f>
-        <v>data</v>
-      </c>
-    </row>
-    <row r="13" spans="3:5" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C13" s="26" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C16" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="E16" t="str" cm="1">
-        <f t="array" ref="E16">_xll.RScript.Evaluate(C16, TRUE)</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C19" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" cm="1">
-        <f t="array" aca="1" ref="E19" ca="1">_xll.RScript.Evaluate(C19, TRUE)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -14985,9 +14911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16A5A11-FD74-4F49-8237-7EB8CA3CF65D}">
   <dimension ref="B2:AJ1110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -24475,7 +24399,7 @@
   <dimension ref="B2:P185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24486,14 +24410,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="O2" s="27" t="s">
+      <c r="E2" s="26"/>
+      <c r="O2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="27"/>
+      <c r="P2" s="26"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D3" s="3" t="s">
@@ -26169,10 +26093,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
@@ -26792,10 +26716,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="E2" s="10" t="s">
         <v>28</v>
       </c>
@@ -27933,15 +27857,15 @@
       <c r="B5" s="10"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
@@ -28634,10 +28558,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="E2" t="s">
         <v>28</v>
       </c>
@@ -29734,10 +29658,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="J2" s="10" t="s">
         <v>28</v>
       </c>

</xml_diff>